<commit_message>
Updating excel file to be a table for sorting/filters
</commit_message>
<xml_diff>
--- a/Challenge 1 - Patient Match/Patient Matching Data.xlsx
+++ b/Challenge 1 - Patient Match/Patient Matching Data.xlsx
@@ -2139,7 +2139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -2269,6 +2269,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2314,7 +2340,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2344,6 +2370,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="19" fillId="8" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="2" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2391,7 +2426,786 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2399,6 +3213,36 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:U202" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="23" tableBorderDxfId="24" headerRowCellStyle="Heading 2" dataCellStyle="Good">
+  <autoFilter ref="A1:U202"/>
+  <tableColumns count="21">
+    <tableColumn id="1" name="GroupID" dataDxfId="22" dataCellStyle="Good"/>
+    <tableColumn id="2" name="PatientID" dataDxfId="21" dataCellStyle="Good"/>
+    <tableColumn id="3" name="Patient Acct #" dataDxfId="20" dataCellStyle="Good"/>
+    <tableColumn id="4" name="First Name" dataDxfId="19" dataCellStyle="Good"/>
+    <tableColumn id="5" name="MI" dataDxfId="18" dataCellStyle="Good"/>
+    <tableColumn id="6" name="Last Name" dataDxfId="17" dataCellStyle="Good"/>
+    <tableColumn id="7" name="Date of Birth" dataDxfId="16" dataCellStyle="Good"/>
+    <tableColumn id="8" name="Sex" dataDxfId="15" dataCellStyle="Good"/>
+    <tableColumn id="9" name="Current Street 1" dataDxfId="14" dataCellStyle="Good"/>
+    <tableColumn id="10" name="Current Street 2" dataDxfId="13" dataCellStyle="Good"/>
+    <tableColumn id="11" name="Current City" dataDxfId="12" dataCellStyle="Good"/>
+    <tableColumn id="12" name="Current State" dataDxfId="11" dataCellStyle="Good"/>
+    <tableColumn id="13" name="Current Zip Code" dataDxfId="10" dataCellStyle="Good"/>
+    <tableColumn id="14" name="Previous First Name" dataDxfId="9" dataCellStyle="Good"/>
+    <tableColumn id="15" name="Previous MI" dataDxfId="8" dataCellStyle="Good"/>
+    <tableColumn id="16" name="Previous Last Name" dataDxfId="7" dataCellStyle="Good"/>
+    <tableColumn id="17" name="Previous Street 1" dataDxfId="6" dataCellStyle="Good"/>
+    <tableColumn id="18" name="Previous Street 2" dataDxfId="5" dataCellStyle="Good"/>
+    <tableColumn id="19" name="Previous City" dataDxfId="4" dataCellStyle="Good"/>
+    <tableColumn id="20" name="Previous State" dataDxfId="3" dataCellStyle="Good"/>
+    <tableColumn id="21" name="Previous Zip Code" dataDxfId="2" dataCellStyle="Good"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2691,97 +3535,97 @@
   <dimension ref="A1:U202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="6" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="6" customWidth="1"/>
     <col min="4" max="4" width="12" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="6" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" style="6" customWidth="1"/>
     <col min="11" max="11" width="15.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" style="6" customWidth="1"/>
+    <col min="15" max="15" width="13" style="6" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" style="6" customWidth="1"/>
     <col min="17" max="17" width="28.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" style="6" customWidth="1"/>
     <col min="19" max="19" width="16.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15" style="6" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" style="6" customWidth="1"/>
     <col min="22" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>594</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>593</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="11" t="s">
         <v>309</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="11" t="s">
         <v>312</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -10406,7 +11250,7 @@
         <v>98626</v>
       </c>
     </row>
-    <row r="193" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A193" s="2">
         <v>59</v>
       </c>
@@ -10441,7 +11285,7 @@
         <v>98626</v>
       </c>
     </row>
-    <row r="194" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
         <v>59</v>
       </c>
@@ -10476,7 +11320,7 @@
         <v>98626</v>
       </c>
     </row>
-    <row r="195" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A195" s="2">
         <v>59</v>
       </c>
@@ -10511,7 +11355,7 @@
         <v>98626</v>
       </c>
     </row>
-    <row r="196" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A196" s="4">
         <v>60</v>
       </c>
@@ -10546,7 +11390,7 @@
         <v>98683</v>
       </c>
     </row>
-    <row r="197" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A197" s="4">
         <v>60</v>
       </c>
@@ -10581,7 +11425,7 @@
         <v>98683</v>
       </c>
     </row>
-    <row r="198" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A198" s="2">
         <v>61</v>
       </c>
@@ -10613,7 +11457,7 @@
         <v>98684</v>
       </c>
     </row>
-    <row r="199" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A199" s="9">
         <v>62</v>
       </c>
@@ -10633,7 +11477,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="200" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A200" s="2">
         <v>63</v>
       </c>
@@ -10665,7 +11509,7 @@
         <v>98626</v>
       </c>
     </row>
-    <row r="201" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A201" s="9">
         <v>64</v>
       </c>
@@ -10685,28 +11529,46 @@
         <v>33</v>
       </c>
     </row>
-    <row r="202" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A202" s="2">
+    <row r="202" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="12">
         <v>65</v>
       </c>
-      <c r="B202" s="2">
+      <c r="B202" s="12">
         <v>201</v>
       </c>
-      <c r="D202" s="2" t="s">
+      <c r="C202" s="12"/>
+      <c r="D202" s="12" t="s">
         <v>529</v>
       </c>
-      <c r="F202" s="2" t="s">
+      <c r="E202" s="12"/>
+      <c r="F202" s="12" t="s">
         <v>591</v>
       </c>
-      <c r="G202" s="3">
+      <c r="G202" s="13">
         <v>40254</v>
       </c>
-      <c r="H202" s="2" t="s">
+      <c r="H202" s="12" t="s">
         <v>33</v>
       </c>
+      <c r="I202" s="12"/>
+      <c r="J202" s="12"/>
+      <c r="K202" s="12"/>
+      <c r="L202" s="12"/>
+      <c r="M202" s="12"/>
+      <c r="N202" s="12"/>
+      <c r="O202" s="12"/>
+      <c r="P202" s="12"/>
+      <c r="Q202" s="12"/>
+      <c r="R202" s="12"/>
+      <c r="S202" s="12"/>
+      <c r="T202" s="12"/>
+      <c r="U202" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>